<commit_message>
Get daily reddit data: Tue Jul 16 08:10:14 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_21.xlsx
+++ b/data/2024_07_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C476"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2981 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1e4j3dt</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>You can never go wrong with red nails!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mltmev3l8ucd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1e4isiu</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Not a professional</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2afxtnx4ucd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1e4iisq</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Robust nail dust collector for manicurist</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4iisq/robust_nail_dust_collector_for_manicurist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1e4i5k6</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>another month, another fill</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg36xnyaxtcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1e4i1qx</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>First time posting here. Not looking for advice, I just wanted to share my set with people I know will appreciate it🖤</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xurxnqm1wtcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1e4i049</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>First time getting chrome or designs. So happy</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4i049</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1e4hyhl</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Grew my nails out twice (All natural)</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4hyhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1e4h8ll</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>My favs🫶🏻</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcm9hadrmtcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1e4h236</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with my tattoos </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrmgwunrktcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1e4g72r</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>I bought this hand bracelet thingy and i just realized how much it matches my nails AHHH</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4g72r</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1e4g3ix</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Look at this chill little dude on my nail</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujq7cgc9atcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1e4fy9n</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help!! Nail glue spilled in my bag </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4fy9n/help_nail_glue_spilled_in_my_bag/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1e4fxsl</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Birthday nails! Sparkly rainbow ombre jellies 💕</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hwvzhmkl8tcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1e4fqui</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Press ons for costume party</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4fqui</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1e4fnbz</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set 💅🏽 </t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzsl2f1m5tcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1e4eo5v</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Should you be buffing nail tips before painting them?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4eo5v/should_you_be_buffing_nail_tips_before_painting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1e4efvz</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Press on nail help</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4efvz/press_on_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1e4ebwq</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Had to shorten my nails and now I'm sad... but at least I have sparkles to keep me going</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4ebwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1e4dvck</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>I found a new (fav) nail tech 👀</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4dvck</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1e4cps4</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>New nail day!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4cps4</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1e4co22</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Ocean Nails</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz1nuop8escd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1e4c43f</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I tell nail tech to not cut my cuticles or dead skin? </t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4c43f/can_i_tell_nail_tech_to_not_cut_my_cuticles_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1e4bvqf</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Press on start up</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4bvqf/press_on_start_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1e4bta7</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Help me not hate these</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fndlj7jr6scd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1e4be57</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>My first time doing nail art!</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu6a0pnb3scd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1e4adl9</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Gel X nails and sensory issues</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4adl9/gel_x_nails_and_sensory_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1e4b2j5</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>leopard print french tips on me by me :)</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cf1dvwl0scd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1e4ay5p</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Day 8 and these press ons are still solid! I've never had them last this long haha </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdz0icelzrcd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1e4awi9</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>any recommendations for nail oil? +new set 🤠</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9g689p6zrcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1e4at3e</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>What brand is the best nail builder curing gel?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4at3e/what_brand_is_the_best_nail_builder_curing_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1e4aiwq</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>First time doing an almond shape! I absolutely love this design!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td1grzsyvrcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1e4afgd</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>My first at-home gel-x set!</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3izy0nk4vrcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1e49rdi</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n46g8pesprcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1e4acsf</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Nail powder keeps lifting on one nail. What can be done to stop this?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4acsf/nail_powder_keeps_lifting_on_one_nail_what_can_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1e491cf</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New York Food Nails </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e491cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1e3ko0n</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Paper thin natural nails?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e3ko0n/paper_thin_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1e48kbd</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>been forever since i’ve gotten my nails done!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k682980dgrcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1e45w1i</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>how can I fix lifting?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e45w1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1e466re</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Gel x issue</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm15dacxyqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1e46u6t</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>I had to go to a different girl today, and I honestly love my nails, the shape looks better in person. But damn she was SO ROUGH, the mark on my pinky is on three other fingers :( a lesson in just waiting to stick w my tech. Does anyone know how long these take to heal?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mj6qjt7j3rcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1e47djr</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Summery soft Ombre Nails with chrome details🌺🥭 (Inspo: @404mast on IG)</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e47djr</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1e47sgf</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Nails I’ve done this year!</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e47sgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1e47roi</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Claws in summer seafoam 🪸🐬🐠🌴</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv1aw7yaarcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1e47n2i</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Question about tanning beds ?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e47n2i/question_about_tanning_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1e477td</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Late birthday nails🫶🖤</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e477td</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1e474d2</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Press on nails….</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e474d2/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1e46r9q</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>update from 200 days ago</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e46r9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1e46ahx</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>flower nails! feel like it fits the summer vibes</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/equpu27ozqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1e4692p</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Kocho Nails</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uderuhrdzqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1e460o0</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>What dip powder brands are the best?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e460o0/what_dip_powder_brands_are_the_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1e45san</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>i'm gonna be devastated when they inevitably break</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sx4m0w4wqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1e45rvd</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Glowy Shimmer Skittles ✨</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e45rvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1e45ocy</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11atjuicvqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1e45d0d</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>My nails tips are clean, but why do they have uneven coloring? How can I fix this? No smoking/obvious causes.</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xia0tx2tqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1e459qb</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>got my nails done today! :3 🍓</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e459qb</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1e457ma</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>I want to get my nails done professionally for the first time. What shape would fit me best? Oval?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bshf4v92sqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1e451zz</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Princess peach set</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvnqkayyqqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1e4501t</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Adorable Press-ons</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32tgu4hkqqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1e44r4y</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Color fading drastically</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e44r4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1e44ck3</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Just did these today ❤️</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e44ck3</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1e44i8o</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Nail sets I’ve gotten so far this year! 🥳</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e44i8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1e44b2j</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did these yesterday </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e44b2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1e44361</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>First time, kept it simple but even my cat loves them</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pslh0x8xjqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1e43rjm</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A few sets I've done on clients </t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e43rjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1e43erz</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Amazing art by @brydiedoesnails on IG!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e43erz</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1e43md6</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>natural nail fail</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e43md6</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1e43oro</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Matte Pink🩷</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12thtqighqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1e43nh9</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cutesy nails🤭 poly gel sculptures </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n26ck5p7hqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1e43f9r</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>obsessed to say the least</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljoupqznfqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1e43d2s</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>OPI 'Another Ramen-tic Evening'</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxqzbk49fqcd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1e43cq8</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>mani with Korean gel products!</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e43cq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1e42qgl</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>2nd attempt at gel x nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e42qgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1e42ktw</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Milky biosculpture 💅🏻</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6mb1rgr9qcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1e42k61</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>$8 press on nails. Not bad!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e42k61</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1e42gmk</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>New Sparklies</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2anqckhy8qcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1e426y1</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i’ve never gotten nail art done! what shape/color/design should i get? </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e426y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1e423rx</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>My newest nails</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e423rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1e41nk7</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>summer look</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e41nk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1e41lym</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Bless the lovely human who posted these press-ons last week 🥰</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e41lym</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1e418vo</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Chrome for summer🦋</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgq57ezb0qcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1e3z73j</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>I’m in love</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3z73j</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1e3xd55</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Fungal Infection - Throw Everything Away???</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e3xd55/fungal_infection_throw_everything_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1e3wdt0</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Is this common?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jj6edc7v1pcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1e40lsy</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My own salon, my own designs. </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e40lsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1e40lfi</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">getting gel extension for the first time, which design would you pick and what price would it be? also - are gel extensions durable? i need them to last a little more than a month </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e40lfi/getting_gel_extension_for_the_first_time_which/</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1e40day</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Selling my Holo Taco Collection </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hos2w4l7upcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1e3zrm8</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Love a sparkly nude!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25zzsja1qpcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1e3zjsk</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>SpongeBob set I did 💅💅</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x82h4vzjopcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1e3z95f</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>[UPDATE] the stickers are the least of my worries…</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3z95f</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1e3yl4w</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Alexa, play Neon Guts by Lil Uzi ✅✅✅</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3yl4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1e3ykux</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Does anyone have filing tips?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e3ykux/does_anyone_have_filing_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1e3yi96</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Rate the manicure for my first client 0/10. Constructive criticism is welcome)</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3yi96</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1e3y4zj</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Birthday nails ✨</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdf626pkepcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1e3y1kr</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">There's something about a classic red! </t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3y1kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1e3xx50</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Still learning but I think I like these</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xhhdbd2dpcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1e3x24u</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Nail art❤️</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft3oz64v6pcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1e3wt0e</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Summer metallic nails</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pbh8xoh25pcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1e3ws8e</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>are these better or worse? rate my progress on the butterfly nails. now ~ march</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3ws8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1e3wpwf</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Advice on shape/color? I usually wear black polish with a rounded edge but I want to change it up!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1tiu65b4pcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1e3wf9p</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Blushing nails 💕</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cri31ud72pcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1e4ibm2</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mercury's Cosmic Tears (video) </t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mctye9t9ztcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1e4dlxr</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Opinions on I Scream Nails?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e4dlxr/opinions_on_i_scream_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1e4d5oy</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Lumen - Glass Stars (May 2024 PPU)</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4d5oy</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1e4d2qd</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Anyone have swatches for this Jen &amp; Berries color?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyc9okvnhscd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1e4cjwp</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Nourishing gel nails that are chip free and long lasting?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e4cjwp/nourishing_gel_nails_that_are_chip_free_and_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1e4c4ic</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>A day at the beach</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60x32shk7scd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1e4c4as</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Island girl nail polish is good</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4c4as</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1e4bvi2</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>looking for revlon divine and foxy dupes</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e4bvi2/looking_for_revlon_divine_and_foxy_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1e4bhdz</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Dry drops</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e4bhdz/dry_drops/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1e4balq</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>New Daveen collection!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/15bi0hr32scd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1e4b4lg</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Nail color suggestions for summer wedding?</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e4b4lg/nail_color_suggestions_for_summer_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1e4b2ha</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>BOLD neon shimmer recommendations</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4b2ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1e49p50</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>"Practice" Magnetic polishes</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/62vlgwy9prcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1e48wta</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>🌅Tequila Sunrise🌅</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e48wta</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1e486mf</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>"Current Events" from Emily de Molly 💚</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e486mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1e4801o</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>The Zoya sale // thisisfine.gif</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kmxbyr2crcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1e47uid</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Avoid Essie Strong Start base</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e89t6c8xarcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1e47ei8</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Late to the 🧲 game</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhv1cwjg7rcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1e4727t</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Recent manis feat Femme Fatale, Emily de Molly, Fancy Gloss and more!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4727t</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1e470po</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Free People Inspo</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e470po</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1e46u83</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>The Lurid hype is so real</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcqx8xcj3rcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1e46oyn</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>A classic-- Mooncat Dragon Scales</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e46oyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1e464bx</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Help!! I’m recovering from nail picking but had a ‘relapse’ and picked off half my gels</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e464bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1e45bqo</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>First time painting and wearing press ons.</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e45bqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1e44tqw</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Indie Polishes - Brick and Mortar Storefronts? </t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e44tqw/indie_polishes_brick_and_mortar_storefronts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1e44mxq</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Experimenting with jellies</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e44mxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1e43xbb</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>So in love with this color!!!!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69akdix2jqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1e43x00</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Is it orange? Is it gold? Is it pink? Is it Caelid? YES</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e43x00</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1e43l16</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>I did the chop!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e43l16</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1e434zl</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>New game: Guess the Inspo!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e434zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1e42aku</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Good Neutral Jelly Polish</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbr8ul0s7qcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1e3yyg2</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>I need help removing the cured glue underneath my nails</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8f1pgk4kpcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1e425b7</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Naiad ✨</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e425b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1e417tm</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>I did pug themed nails to celebrate picking up my new puppy</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e417tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1e40ojl</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Some polishes just can’t be photographed!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e40ojl</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1e40iyf</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Hot pink on a hot summer day ☀️</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlls3recvpcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1e3zehb</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Help looking for anniversary gift for wife</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e3zehb/help_looking_for_anniversary_gift_for_wife/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1e3ymy7</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Gangsta Boo dupe?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3ymy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1e3ym0p</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Magical ethereal nails</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yw6wu7fvhpcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1e3xr3t</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Summery soft Ombre Nails with chrome details🌺🥭 (Inspo: @404mast on IG)</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3xr3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1e3wwik</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Summer metallic nails</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/907jyxjr5pcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1e3wr14</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer - Evolve Today</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3wr14</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1e3we1z</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Metallic Fruit Skittle 🍊</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3we1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1e3vs1y</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you guess this red by looking at it? It’s my favourite vampy red of all time. </t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wfgez2dxocd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1e3vrrx</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Ridgey laqueristas: your favorite ridge fillers for truly effed up nails.</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4r434nraxocd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1e3veg1</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Neon shimmer ✨</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w30blf5iuocd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1e3v9ww</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Does this nail shape suit me?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1ek144jtocd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1e3v83k</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Has anyone ordered from Nailtique’ s website recently?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e3v83k/has_anyone_ordered_from_nailtique_s_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1e3ukp8</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Mercury's Cosmic Tears</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3ukp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1e3u0v3</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Small Stupid Humans</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3u0v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1e3tugm</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Tie dyed ✌️💅</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3tugm</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1e3trfx</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Zoya - Kira 💙</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3trfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1e3r1hn</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e3r1hn/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1e3qndj</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">High Society 🚬 </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3qndj</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1e3pqua</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails french manicure </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3pqua</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1e4ifcb</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Guess the background is real??</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e4ifcb/guess_the_background_is_real/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1e4gs4t</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Some summer fun</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4gs4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1e4ggd0</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>🍋🍋🍋</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbrax3l0etcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1e4fw5l</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Birthday nails! Sparkly rainbow ombre jellies 💕</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hb7xg0n48tcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1e4eoq0</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e4eoq0/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1e4dtzd</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>My favorite set so far. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2hmkp9ioscd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1e4ao2j</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Finished my pink cheetah print angel press ons 💕</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft4iief4xrcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1e4898b</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black water like design </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw7a5fyzdrcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1e4715x</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>˚ ༘ ⋆｡˚✧Fruity Summer Nails ✧˚ ༘ ⋆｡˚</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lltf61yu4rcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1e46dcv</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Love these</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arorgte80rcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1e4303s</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I had to do something a little bit fancy for one of my favorite Pokémon. </t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn3x4auscqcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1e424t7</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i’ve never gotten nail art done! what color/shape/art should i get for my first time? </t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e424t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1e3xpxh</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Fruit nails</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3xpxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1e3xd5y</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>They Look Like Cookie Icing To Me 🍪🤍🌟</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3xd5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1e3x5mz</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Blue textured and ombre nails</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdqwjpzk7pcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1e3wsls</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Hibiscus neeeds work</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3wsls</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1e3wnl8</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>progress(? on the butterfly nails</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3wnl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1e3twu6</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>DIY 🦓 recreation 🩷</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3twu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1e3t98l</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>My beginner nail art :P</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3t98l</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1e3pgii</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>How do you rate my new work? 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e3pgii</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul 17 08:09:15 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_21.xlsx
+++ b/data/2024_07_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C476"/>
+  <dimension ref="A1:C628"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8525,6 +8525,2590 @@
         </is>
       </c>
     </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1e5co6m</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Beautiful natural toes😍 Cr: Thee_Celeste</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3neq2dmd1dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1e5c2sz</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>I think white with chrome will be my new go to 😍</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uxedw4561dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1e5bovq</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Damaged nails</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87sp3nbl11dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1e5blhl</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Decades later and I still can’t seem to find a way to open shit without damaging my nails 🔪🔪🔪🔪</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5blhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1e59nxr</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>My Nails artist suggested a different chrome and I'm glad she did!!!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e59nxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1e5928v</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can never go wrong with rhinestones 💕 </t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46sf6xtz80dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1e58z2k</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Vixen by Revlon - What is a good dupe?? It’s my favourite.</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skj0lwv480dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1e58xw3</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd Gel X attempt!! So far the best </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e58xw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1e58oxi</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I keep this set forever? </t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyp18l2g50dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1e56323</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Does anyone else here use nail wraps?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3on1zpmhzcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1e57wg7</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | CHI S*xy Bish</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e57wg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1e57q0d</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Nail shape?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e57q0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1e57n90</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer set. </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e57n90/summer_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1e57gpf</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e57gpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1e57atw</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new set 🪽 </t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e57atw</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1e576ou</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of this nail shape and color? </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/466gk3p9rzcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1e575e8</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Lemming Lacquer - Grimm Adventures</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e575e8</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1e56xfj</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>This colour combo though 🧿🪬💎</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e56xfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1e56xb1</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>This colour combo though 🧿🪬💎</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e56xb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1e56nfk</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>I don’t know why but this nude glitter has me in a chokehold 🤩</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra2y0qukmzcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1e56j3h</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Watermelon Fun!</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quavyq2ilzcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1e56frn</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Shiny nails for me, I love glitter nails</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1b7vxnpkzcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1e55ot8</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Short nails</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e55ot8</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1e505ph</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Taylor Swift Lover inspired nails 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na3hosy26ycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1e54jv9</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Cat nails 💛</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu26490i4zcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1e5476p</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Love this simple look</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gaoe9bqk1zcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1e542pc</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Birthday nails ✨️</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e542pc</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1e53zdm</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>this months nails 🥰</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4372kwrzycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1e53lc8</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>HELP I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e53lc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1e53iqd</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>My first time doing nail art!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klibrs80wycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1e511vt</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>My cottage core inspired press-on set</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e511vt</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1e533ql</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Is it normal for acrylic nails to grow out uneven like this?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6swr2z9psycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1e52ztv</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>One nail broke and all the rest had to go with it 🥲 but i kinda like it and everything looks pretty with this green!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e52ztv</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1e52jbs</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail tips WILL NOT stay on. Any suggestions? </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e52jbs/nail_tips_will_not_stay_on_any_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1e52595</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Need a nail polish organizer for a desk drawer</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e52595/need_a_nail_polish_organizer_for_a_desk_drawer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1e51e5d</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>French tips but make it glittery!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ce9lwrdfycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1e50swk</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Needing advice - need nice nails for a month or so, have never had fake or long nails </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e50swk/needing_advice_need_nice_nails_for_a_month_or_so/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1e50m83</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmocnscg9ycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1e50fjd</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>I love how my new set turned out! (My work)</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tflg40y18ycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1e50dn2</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Fruit stickers done by myself</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e50dn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1e50a2l</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e50a2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1e507ud</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Bright red</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3ta84ei6ycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1e4zuwk</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red Nails! </t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4zuwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1e4zv6d</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I pull off almond? </t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pknae3nx3ycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1e4z8dx</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Do the fellas get their nails done too</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0jz5gzczxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1e4z67b</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Gel polish again for the first time in months</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzg1b9ixyxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1e4ypqe</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Vacation Nails</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1652yyxlvxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1e4yp1n</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Can you tell where I’m from based on the colors?!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9cj9lmgvxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1e4yp1i</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>French and chrome combo 🩷</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nvaaysgvxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1e4yob1</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bad at taking pics but wedding nails!! </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4yob1</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1e4yjpp</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>painted these a bit ago (i miss them)</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4yjpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1e4yaag</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Practice will eventually make perfect!!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2v525rzhsxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1e4y8wq</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Did my moms nails</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4y8wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1e4y2ve</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>DND 760, bright orange what do we think?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6aiekvyqxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1e4xu5q</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>I LOVEEEEE THESEEEE</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyhxwwl7pxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1e4xrcw</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">¿Most flattering Nail Shape? </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4xrcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1e4x4pp</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>hand sculpted rilakkuma nails 🧸🍓💛 look at korilakkuma holding the strawberries omg! all hand sculpted 💕</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4x4pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1e4wttv</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Went to Casa de Toddler and got a free mani</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksfqdo3vhxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1e4w693</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>After seeing a couple of posts about these press-ons I had to try them - did not disappoint!!!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4w693</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1e4w41f</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Can I grow my nails into an almond shape? The sidewalls are wonky and my nails always grow into trapezoids</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4w41f</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1e4usn6</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer nails! 💙 I’m happy w them </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1o48srt53xcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1e4ubj6</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Double base coat?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4ubj6/double_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1e4uimg</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Natural nail growth</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ii15z461xcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1e4s267</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>How to ensure my nails won’t break</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4s267/how_to_ensure_my_nails_wont_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1e4r8cv</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Looking for some advice!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4r8cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1e4pbfj</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Original seller for the fake/acrylic nail rings?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4pbfj/original_seller_for_the_fakeacrylic_nail_rings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1e4u68j</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My colorful new set 😍 </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4u68j</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1e4torq</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>All natural nails, they do chip a lot as you can see from the different lengths.</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4torq</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1e4tavr</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Men’s nails- help</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4hdbgoiswcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1e4t5y4</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>first time nail questions!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4t5y4/first_time_nail_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1e4sffr</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Nails for NYC Trip</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4sffr/nails_for_nyc_trip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1e4s1ru</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Ombre press on Nails</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cs1uclcmjwcd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1e4rv51</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>was struggling doing pushups @ the gym, but couldn't help to stop &amp; admire how my nails looked on the mat -- it's the little things🤭</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4rv51</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1e4rrpg</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sea nails </t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b60uck3khwcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1e4r8jy</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Another nail tribute in memory of my sweet girl 💓🦋</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4r8jy</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1e4pvly</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Cherries for summer 🍒</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0rh84tt3wcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1e4ptpl</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Neon Fun</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4ptpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1e4p4y2</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>The most extra nails i’ve ever had</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4p4y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1e4ogb0</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Has anyone tried PolishPops?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4ogb0/has_anyone_tried_polishpops/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1e4odm9</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>I want to learn how to do my own acrylics. What amazon set should i buy?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4odm9/i_want_to_learn_how_to_do_my_own_acrylics_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1e4nyay</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Sonne shape examples i did recenrly for to practice. Feedback very Welcome.</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4nyay</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1e4no8h</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>latest UV gel look: 2 coats funny bunny &amp; 1 coat bubble bath OPI</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4no8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1e4ncpc</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Feedback please!!!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4ncpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1e4my1q</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vz9spnpufvcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1e4mxzi</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Rhinestones... 🥰</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66fvhrptfvcd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1e4mesx</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>French Pedicure</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4mesx</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1e4mdqg</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For graduation </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4mdqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1e4ln48</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Yipeeee</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u24252fx2vcd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1e4l4ss</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>What is that glue that is used for nail art but you put it on your skin? then peel off so the nail polish isn't in your skin?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4l4ss/what_is_that_glue_that_is_used_for_nail_art_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1e4i9o3</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Help! Why is my 3D gem (made from topcoat) going cloudy/matte when secured onto the nail? (Also with topcoat)😢</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weypi9bmytcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1e4hxp3</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Nail chipped after 4 days</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4hxp3/nail_chipped_after_4_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1e4k1yz</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Can regular nail polish and gel products be used together?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4k1yz/can_regular_nail_polish_and_gel_products_be_used/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1e4jrcd</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>freestyle question</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e4jrcd/freestyle_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1e5awjs</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>How did they turn out, these are my first nails</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7wkl0tfs0dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1e5aaxl</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Our Princess is in Another Castle</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5aaxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1e59zo5</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with soft nails and gel application </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e59zo5/help_with_soft_nails_and_gel_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1e597ev</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Refreshed an old mani with a magnetic 🤩</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ts40zjqda0dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1e587ep</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Secrets of the Sea from Arcana Lacquer!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ca4qv8uo00dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1e57ylc</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | CHI Sexy Bish</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e57ylc</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1e572i4</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Lemming Lacquer - Grimm Adventures</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e572i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1e566yl</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Barbie Nails for Summer ☀️👙💓</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qt4sg1kizcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1e55wz8</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help - can I lightly file a structured gel manicure to reshape at home? </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e55wz8/help_can_i_lightly_file_a_structured_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1e55sny</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>What PBE overpours are y’all getting?!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e55sny/what_pbe_overpours_are_yall_getting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1e55d56</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glow in the dark Electric Daisy by cirque colors </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e55d56</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1e54u5t</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>After years of going to the salon, I’ve started doing them myself again. Definitely not like riding a bike 😅</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e54u5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1e54da6</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Potion Polish 😍</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6c8wjvy2zcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1e54acq</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Solar Color Dust pigment mix-in advice?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e54acq</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1e51cya</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>help me find an essie shade</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udfowkv3fycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1e4vrje</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Lurid skittle 🩷🧡💜</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4vrje</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1e52wha</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Loving ‘Chemical X’ from Mooncat!</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjw8y915rycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1e52st5</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Little summer polish roundup!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e52st5</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1e50k9u</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is my Sin Eater evaporating?? </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e50k9u/is_my_sin_eater_evaporating/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1e504r8</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>i get the magnetics love now</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e504r8</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1e4zp6m</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>YNNB success [gel + regular polish]</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9r0rgyco2ycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1e4z78w</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Been sitting on this one for 2 and half years</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4z78w</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1e4ylch</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>I tried to dupe “Aperol Spritz Anyone?” by LightsLacquer</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4ylch</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1e4ygzh</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas vibes in July 🎄 </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0y758kttxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1e4y4aq</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For my fellow glow-the-dark lovers </t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqezbcxarxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1e4w3tf</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another summer manicure! </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4w3tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1e4vwru</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Mooncat's Forces of Evil on top of Merkitten</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1o4eeh8bxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1e4vptu</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>??? i’ve bought three glossy top coats and they do the same thing??</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jojix9yv9xcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1e4vlhj</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Dew Polish Blossom</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4vlhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1e4vejv</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Anybody try to paint their nails while in a cast for a broken wrist?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e4vejv/anybody_try_to_paint_their_nails_while_in_a_cast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1e4v5re</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Holo &amp; henna - what do we think?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9zr1h8s5xcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1e4si2j</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Here Lies Hopes &amp; Dreams</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4si2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1e4sb8k</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Summertime shimmer! 😍</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4sb8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1e4sak8</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>You Hooooo!!!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/02xdgbielwcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1e4s0pd</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Cactus Jelly + Poparrazzi Glass Ceiling </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc6r3wjejwcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1e4rvx4</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>This gradient reminds me of this fish emoji 🐠</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4rvx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1e4ru2c</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>I’ve had this for only 1.5 years. Does this mean it’s gone bad?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnnsgny1iwcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1e4rey6</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>ABCs of polish! T is for The Don Deeva</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw69uf1zewcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1e4nsvn</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>🎮🍄It's-a-Me!🍄⭐️</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4nsvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1e4n42b</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>I always forget how much I love Shooting Star until I pull it back out 💙💜</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4n42b</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1e4loll</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Rubber base</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4loll</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1e4kopo</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>A UK dupe for Cirque Cloud 9?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4kopo</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1e5ck42</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>beautiful nails ❤️</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f14ous69c1dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1e5cj78</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>delicate nails 🥰💖</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvknirhxb1dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1e5asmd</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>I didn’t realize how messy the gold mirror gel would be 😭</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y5fbkaar0dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1e55kn5</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Nails princess by me @streetnailart ✨</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y81onn18dzcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1e521cg</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tulips!! </t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8or2eqdckycd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1e4zf1e</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>how can i improve? i have trouble with making them look refined and clean (natural nails)</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4zf1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1e4yrx7</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first attempt at a gel french manicure </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4yrx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1e4yqni</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Vacation Set</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10dydotsvxcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1e4x5uq</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Hand sculpted 3D Rilakkuma and Korilakkuma nails!💛🍓🧸 look at the little strawberry charms omfg!😭🍓🧸</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4x5uq</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1e4x3bd</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Flame Grilled! 🔥</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4x3bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1e4x09t</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>What polish is your favorite?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e4x09t/what_polish_is_your_favorite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1e4uma7</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Heart on my sleeve err hand?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvkkdrmw1xcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1e4ukkm</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>How is my my nail polish?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmscjm0i1xcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1e4s78h</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>The design with ring included</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91z9tuwpkwcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1e4rrn8</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Sonne shape examples i did recenrly for to practice. Feedback very Welcome.</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48u2zgdihwcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1e4pb7l</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Dreamy chiffon ribbons</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4pb7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1e4jjk0</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>what do you think of my work? @koku_lacquer on ig btw!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e4jjk0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul 18 08:09:18 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_21.xlsx
+++ b/data/2024_07_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C628"/>
+  <dimension ref="A1:C789"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11109,6 +11109,2743 @@
         </is>
       </c>
     </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1e65hou</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Abstract nails</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyrac46mb8dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1e650bq</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>My new set of nails🥳</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wh96k4u58dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1e64z3l</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Fifth set</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e64z3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1e64wyh</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Each nail gets to wear a pretty outfit!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mexpesn48dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1e64noz</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Shiny white nails</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e64noz</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1e64j3a</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer Nails 💅 </t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o4ncex9108dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1e64h44</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>My fourth set</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e64h44</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1e5zky7</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>What do I need to make my own fake nails at home?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5zky7/what_do_i_need_to_make_my_own_fake_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1e61abk</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Dupe for Chanel Vamp</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e61abk/dupe_for_chanel_vamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1e62ukt</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Nail snapped off less than 2 weeks, is this normal?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e62ukt</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1e63yco</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite UV gel base &amp; top coat? </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e63yco/favorite_uv_gel_base_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1e63rkw</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Hahaahaa Laugh with me</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e63rkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1e636sy</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Set 😝 </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ii5hf62ok7dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1e62ugj</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Cuticle remover -&gt; nail lifting?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e62ugj/cuticle_remover_nail_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1e626ch</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Whale of a time</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f997q3dea7dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1e621no</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>No to the gel mani</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e621no/no_to_the_gel_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1e61sg3</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>No Negative Vibes PressOns</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e61sg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1e61e9l</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Stars and chrome</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e61e9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1e5zr92</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Nail Rhinestone Glue Question</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5zr92/nail_rhinestone_glue_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1e5z0b2</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>I feel like Carmela Soprano.</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5z0b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1e60wvd</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Structured gel </t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xpxhm27gy6dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1e60oo2</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>gel x!!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e60oo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1e60gnq</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kiyhpryau6dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1e604gd</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Seashells 🐚✨</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e604gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1e5znv5</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1h4ohj3n6dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1e5zid1</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thsljuuql6dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1e5zg9r</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Late pictures, but I wanted to show you all! </t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnqfge18l6dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1e5z3zn</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>I designed the box, my sister designed the nails, aren't they beautiful?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5w8jyjci6dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1e5yr32</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>I tried something different today!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5yr32</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1e5yf1b</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Beach Vacation - gel or regular mani?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5yf1b/beach_vacation_gel_or_regular_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1e5y752</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Got acrylic’s for the first time! They match my eyes and glasses,</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5y752</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1e5xxp1</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just started doing my own gel nails and trying designs. How can I improve my skills? </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5xxp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1e5x3e7</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>My Baby Shower Nails 😍🩵</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4mh3vd816dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1e5x295</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>My first time using solid glue for press on nails. Someone disapproves.</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltb9ksol06dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1e5wwrx</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Looking for a hero!</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5wwrx/looking_for_a_hero/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1e5wv6u</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Water and Gel Polish</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5wv6u/water_and_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1e5wqgl</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Recent sets, self done</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5wqgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1e5wcd9</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kuromi nails :3 </t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1brndv87v5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1e5vuac</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b07x6der5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1e5vjxy</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Aquamarine vibes 🧜‍♀️🩵</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5vjxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1e5vb4s</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Should have tried sheer gel nails sooner!</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rw68gtfcn5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1e5v9e5</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My client took this perfect photo of her nails herself </t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4nj7qqym5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1e5v3rp</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feelin’ groovy 🧡💜credit to Esthetics by Katie. </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtb5zkfrl5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1e5uss4</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>How to grow my nails faster?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5uss4/how_to_grow_my_nails_faster/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1e5u8c0</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>baby shower nails :)</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5u8c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1e5u6x8</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Silver foil with a red coat on top</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svzc8u83f5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1e5sfkl</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Salon did my manicure but I am not 100% happy</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5sfkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1e5tp8o</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Been doing my own nails a couple months now</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nik3getib5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1e5to7f</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>new pearly nails!</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr6o08z9b5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1e5sxn1</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>☀️ ILNP Brightside 🧡💛</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5sxn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1e5qlq4</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>What services are ya'll choosing to avoid thicc looking nails?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5qlq4/what_services_are_yall_choosing_to_avoid_thicc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1e5rlgu</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>My wedding nails💐🌿</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgylm7w0w4dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1e5r2p5</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Festival ready🧡🩷</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5r2p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1e5rtfe</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech wanted to experiment today. </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwt5f6dkx4dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1e5r62v</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>New set ‘Punk’ part III</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhav1b8vs4dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1e5qkbx</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Is it normal for one persons pedicure to take 15+ minutes longer than the other?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5qkbx/is_it_normal_for_one_persons_pedicure_to_take_15/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1e5pjl5</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Possible solution to press-on nails for club thumbs...</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5pjl5/possible_solution_to_presson_nails_for_club_thumbs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1e5pm6q</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Tutti Frutti</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1aek8annh4dd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1e5knbn</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Breaking Up with Dip-- Help Me Choose??</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5knbn/breaking_up_with_dip_help_me_choose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1e5n3a4</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>trying to get better!</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5n3a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1e5pkhw</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>I've been eyeing this colour for months and I finally got it 💜</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5pkhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1e5pbsl</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>My handmade press on nails 🦋</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgaow8qjf4dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1e5p9v2</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Gel nails after “ring of fire”</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frrl3r76f4dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1e5os11</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>A little sparkle and shine ✨️</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5os11</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1e5o3kj</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Pedicure nail art</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5o3kj/pedicure_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1e5o299</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The pointier the better is my nail motto </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5o299</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1e5nju7</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>my summer nails</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5nju7</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1e5nhuw</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Road to repair my nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g72b6u8e24dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1e5n7fn</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Purple gradient sparkle.</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lui98j6d04dd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1e5m6jj</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving my most recent colour choice </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b19cblys3dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1e5klsr</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>I used to be a nail biter, and I had almost no nails. After many times of trying to stop and failing, I finally succeeded and have had my nails long for about half a year now. These are my natural nails with gel polish. 😊</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkvt4qgkh3dd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1e5ker4</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>New set ‘Punk’ part II</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5ker4</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1e50rqb</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Question for my nail techs - how to give constructive criticism.</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e50rqb/question_for_my_nail_techs_how_to_give/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1e55bou</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Help - can I lightly file a structured gel manicure to reshape at home?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e55bou/help_can_i_lightly_file_a_structured_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1e5c8mk</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>How to Fix a Ripped Nail? Help??</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afaf2jn681dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1e5k2ei</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Crocheted Nails. Are they realistic enough to fool people? </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tomh0jcqd3dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1e5jyyi</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>I did my own nails and I'm a beginner, how much would they charge these in the US?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5jyyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1e5i67s</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Gel-X Nail for wide nail beds</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5i67s/gelx_nail_for_wide_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1e5isvp</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Short thumb nails </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5isvp/short_thumb_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1e5jpbc</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>new nails done by myself!🐬🌺</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr4wn0j1b3dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1e5j55v</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>New Sparkily manicure. Feedback please 🫶</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5j55v</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1e5hnr5</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Gradient Peach Nails 🍑</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5hnr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1e5hcq7</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mushroom Nails </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7na2ihd8s2dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1e5gnj8</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>ILNP - Enchantment</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/crk6huwvl2dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1e5gcck</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5gcck</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1e5g2kg</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Stars and sparkles, my emo adolescence is still here😂</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3dl34neg2dd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1e5fv5x</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>new set ☺️💞🌸</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k8d843mde2dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1e5fl0g</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Tried a purple-milky fade and am super happy with the result</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44f48gsgb2dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1e5fiir</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Sad day, it’s the worst when one breaks 😭</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3treo9ypa2dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1e5ff57</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>My second time doing nail art!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2b70f2s92dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1e5e6l7</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>New to nails - help!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5e6l7/new_to_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1e5dwkn</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Cherry Red PVC Nail Extensions</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqv4v5nps1dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1e5dkvy</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Nail hack…..</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5dkvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1e5d51i</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>How can I grow my nails?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5d51i</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1e5d3b7</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Old nail set</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i6vya3si1dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1e5d0o8</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Has anybody know this company??</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e5d0o8/has_anybody_know_this_company/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1e647aj</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Give me your pickle Shrek green</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e647aj/give_me_your_pickle_shrek_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1e63qx2</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Orly Color Pass for Fall is gorgeous. (Not an ad, just someone who uses their subscription.) </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9y1qt69vq7dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1e63a9a</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Nail polish noob here. Can this dent be easily fixed?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8hqhg7ql7dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1e62lgm</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Anyone having issues with Lights Lacquer bottles cracking and breaking like Mooncat?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e62lgm/anyone_having_issues_with_lights_lacquer_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1e5ybpn</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>OPI - You Don’t Know Jacques dupe</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e5ybpn/opi_you_dont_know_jacques_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1e5zqmt</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Seashells by the Seashore ✨</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5zqmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1e5ylsu</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>👽 Polishes Used: Cirque Colors (Shade: Earthen) | Essie (Shade: Good To Go Topcoat)</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5ylsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1e5ylgr</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>🍉 💀</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5ylgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1e5ykqv</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Midnight Fireworks (and lots of rainbows)</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5ykqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1e5yk5o</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Belated Pride part two! 🌈</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5yk5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1e5yh5w</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>🌈 I’m a bit late on posting, but happy Pride everyone!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5yh5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1e5ycjg</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>🎀 Polishes Used: Cirque Colors (Shade: Coquette) | Essie (Shade: Good To Go Topcoat) 🎀</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5ycjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1e5y44t</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You greedy little dirtbag </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5y44t</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1e5y04u</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Decided to inspect my recently purchased Mooncat bottles. Does this look like a crack to you?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5y04u</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1e5xa1z</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Non-holo dupe for Cirque's Scorched Sorceress? </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cf5ba6q26dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1e5wrua</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Cirque Colors Spa Water!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i7jlj5emy5dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1e5wmfp</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Probably my favorite combo</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5wmfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1e5vwxo</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Think I found my perfect red 😍</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5vwxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1e5vvfy</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh n clean gel set this week (gel ombré) </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kktj6dpmr5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1e5vksv</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>🫧🫧💀</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5vksv</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1e5urg8</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Mother of pearl inspired</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d23j6p2aj5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1e5vjh3</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>You Greedy Little Dirtbag</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q72qt2c4p5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1e5vajz</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Cat approved polish</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5vajz</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1e5v6na</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Shipping nail polish to or from or within Canada ?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e5v6na/shipping_nail_polish_to_or_from_or_within_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1e5us59</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Warning eating trolling night crawlers may cause bitten fingers!</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5us59</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1e5upm3</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Happy Mail Today!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4iif2otui5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1e5uddf</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Shout out to my funky finger friends! Getting an elegant photo can be so hard 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifwq2upfg5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1e5sx1o</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>☀️ ILNP Brightside 🧡💛</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5sx1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1e5sp70</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>🐭🧀Cheese🧀🐭</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5sp70</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1e5qqpd</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>First Ombre</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5qqpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1e5q4kb</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>how sparkly do you want it? YES✨</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gy4thw4bl4dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1e5p4n9</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Strawbery milkshake inspired 🍓</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06lrs4s3e4dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1e5oao7</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Secrets of the Sea by Arcana Lacquer </t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5oao7</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1e5oa8l</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Just got my Cirque Birthday Sale order and wanted to share 💙🧡</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5oa8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1e5o1uh</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>pink lemonade 🩷🍋</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4cofqld64dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1e5ndcs</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hey Google, set a timer for 90 minutes </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5ndcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1e5m6az</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>{Gifter PR} Look what I got 👀 (repost)</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcx2yn4ws3dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1e5m5jp</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Magnetics are a headache!</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/embulq1rs3dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1e5lb22</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>I call these sparkly shrek nails✨</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5lb22</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1e5k6cw</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Feel like I have jolly ranchers on my hands 😍</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5k6cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1e5is37</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>The obsession begins! Any critiques or general advice?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5is37</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1e5i5w7</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Body Glitter Experiment 🧪 💅</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5i5w7</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1e5gmei</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP - Enchantment </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/adqyu60ll2dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1e588vo</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for inserts for my Alex drawers </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://a.co/d/irOrbiH</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1e5atba</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Got my regular polish to last 3 weeks no chip with this hack</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sscm8o3hr0dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1e56vmu</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Obsessed with magnetics lately</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a5oeipplozcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1e545ub</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>I am a novice at doing nails/ nail art. This is the first set I'm 100% happy with and proud of. It took me over 5 hours. 3d bug nails!!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e545ub</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1e5d6cg</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Cirque Colors Dove Jelly &amp; Spotted 🩶</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5d6cg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1e649i2</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Proud of myself 😁</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e649i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1e625at</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing butterfly wing design </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e625at</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1e61fap</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t59dak9437dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1e606zn</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Do you like the color?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yv1wiydor6dd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1e5zq9k</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Rhinestone Glue Question</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e5zq9k/rhinestone_glue_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1e5z4e0</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Hello girls, I'm looking for nail ideas that are coffin-type and light in tone 💓</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e5z4e0/hello_girls_im_looking_for_nail_ideas_that_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1e5wflc</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kuromi nails &lt;3 </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5wflc</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1e5urc1</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Purple Plants</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3upin1y8j5dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1e5s005</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Tips on using silver chrome gel?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4xwimtwy4dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1e5r8lz</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alaskan cruise nails </t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5r8lz</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1e5q283</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>beautiful nails ♥️✨️</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8u6yw7uk4dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1e5o3ve</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>My tattoo makes this look so fun. Did my nails myself !</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9scvlbzr64dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1e5m9q7</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Finally tried the trending 3d flower 😍</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7avae59lt3dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1e5le7v</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>My Coworker was suuuuuch a real ass bitch and let me do her nails</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e5le7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1e5jjbc</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkb3g49s93dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1e5hivv</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How it's looking </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wm99hynpt2dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1e5e0fg</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Gold Insect Decals</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8h6k81oxt1dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jul 19 08:09:10 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_21.xlsx
+++ b/data/2024_07_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C789"/>
+  <dimension ref="A1:C950"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13846,6 +13846,2743 @@
         </is>
       </c>
     </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1e6xxjf</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Spanish nails?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6xxjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1e6xlox</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>How to get rid of bumps in gel polish (uv/led) ?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6xlox</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1e6x5r0</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Froggy nails🌼🐸</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6x5r0</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1e6wzak</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Ripping acrylics?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6wzak/ripping_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1e6ww19</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>gel manicure grow-out</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6ww19</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1e6wrtq</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>My husband hates it</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8u1qwea33fdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1e6wahp</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Fruit nails pt 2 :)</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljsyckcixedd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1e6w06y</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Nails I just did!</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6w06y</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1e6vuke</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>I was feeling chromey 💕</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5krwrlisedd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1e6vmyk</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Which shape do you prefer?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6vmyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1e6virt</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying ombré nails with acrylic </t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8osi65yoedd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1e6tunl</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>i got gel for the first time; this bubble keeps getting bigger. is it an allergic reaction or just rushed technique?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mejv1tmw7edd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1e6v5wi</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Powder nails on my honeymoon </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6v5wi/powder_nails_on_my_honeymoon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1e6v0fm</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Peep the new set🤪</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukk1wnpkjedd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1e6usi4</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Too soon to get nails done again?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6usi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1e6t6yd</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Can I put a clear gel top coat over shellac nails? What about over regular polish?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goywqask1edd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1e6ufgp</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>$125 russian hard gel manicure. was it worth it</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6ufgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1e6uaw6</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Male Nails</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6uaw6/male_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1e6u4q7</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Go pink or go home 🩷</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze7fwejlaedd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1e6t0h5</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Drippy Goth Tips</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6t0h5</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1e6swy1</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Should I get this fixed professionally?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq5rwby0zddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1e6si0s</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How much do they give to my nails from 1 to 10? 🪬💅🏼 </t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq3m41t5vddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1e6s4ew</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>What is happening with my nails?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6s4ew</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1e6rpvd</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Help: acrylic nails not coming off! I cut them down, soaked in warm 100% acetone for over thirty minutes, and used a cuticle pusher to gently work them off. Feels like they were bolted on haha</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6rpvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1e6pxzv</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Help me find this colour 💜</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6pxzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1e6oyvv</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>new extensions! didn't cut my natural nails beforehand ...</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6oyvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1e6n4j1</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t even know where to begin and what to do with them </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6n4j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1e6twrl</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Can these be fixed?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6twrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1e6md9z</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>$3  press ons🫢💗</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7x6f35efcdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1e6m66t</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>nail tips needed!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pft196jwdcdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1e6l6d8</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Sometimes, I let my daughters chose my nails and they get theirs painted the same way.</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6l6d8</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1e6szhm</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Friendly PSA that boys need to get nails too</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6szhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1e6s9mv</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Guess my idea</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7x2efi40tddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1e6rbkv</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Paint Lab…least fav so far 🫤</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6rbkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1e6r5x6</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Is this normal growth for 2 weeks?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htaao0zyiddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1e6qo14</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>heart tips</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6qo14</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1e6qhaz</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>press ons with added nail stickers!</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhvrm28scddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1e6plku</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>3rd attempt at gel x and nail art</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t78zk23d5ddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1e6os1v</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Which brand has the absolute shortest of SHORT nails?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6os1v/which_brand_has_the_absolute_shortest_of_short/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1e6oof1</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>A few of my favorite/craziest sets</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6oof1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1e6ojqw</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Nails💅🏻</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6nrrctuwcdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1e6odoq</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Ombré sparkle</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmzb038lvcdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1e6o8fq</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>My dip nails always look so thick from the side, what can I tell the tech to avoid this (dip nails)</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6o8fq</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1e6nhzv</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Anyone a fan of this color...?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h13b1ccxncdd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1e6mii5</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whatcha think for my first time doing my nails? </t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6mii5</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1e6mazy</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my favorite nails </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uzt4t0xecdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1e6m9aw</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>French tip chrome finish</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6m9aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1e6lzsr</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>IBD UV/LED Bonder</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6lzsr/ibd_uvled_bonder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1e6lsrp</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>What to ask for at the nail salon ?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6lsrp/what_to_ask_for_at_the_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1e6lqd5</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>I painted my nails for the first time in a while.</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24c3n1bnacdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1e6kyco</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Got my first press ons today</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6kyco</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1e6kiv5</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Antique vibes</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9r4p5mr1cdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1e6iqwx</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations for hypoallergenic gels/polishes? </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6iqwx/recommendations_for_hypoallergenic_gelspolishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1e66sxb</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>What is going on here???</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e66sxb/what_is_going_on_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1e6jua2</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>🍑</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/av2yxe7nwbdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1e6k4ha</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Anyone else like using nail and gel polish together?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq77xctqybdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1e6jfxm</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>A little color for summer 🌞</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e6eggentbdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1e6jcpz</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>my nail technician does a very nice job🤩</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6jcpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1e6j04p</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of polygel toes </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq5qnj4kqbdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1e6iwex</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Not usually one for pink but…</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpqkv0sspbdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1e6ipcn</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>White with Unicorn Chrome🦄</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5o1putdobdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1e6il17</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Testing out wedding nails! Part 2</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dv3xphmjnbdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1e6icw2</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>This is my favorite set so far!</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv9oo3xxlbdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1e6i85l</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>My wedding nails 🤍</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6i85l</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1e6i7xk</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>My wedding nails 🤍</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6i7xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1e6i3is</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>DIY “fill”</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tl2pn6v4kbdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1e66k7c</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>how i make my press ons last 2+ weeks</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e66k7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1e670oh</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>What I got vs what I asked for :) inspo found on Google but I traced it back to another redditor on here! mine were done at a shop in Woodbury, MN</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e670oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1e676lj</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strawberry soda inspired 🍓 </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8tu8qp5x8dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1e6a442</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Was inspired by a pic on seen here</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6a442</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1e6ezl1</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Summer nails, baby!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l74a8ex9vadd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1e6fs6q</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Gel-X for durability (not length) only?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6fs6q/gelx_for_durability_not_length_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1e6gvz4</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Wanted something simple but fun</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1na5xvz9bdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1e6gii4</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>New sparkly pink nails for the summer!!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s398cpn77bdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1e6gaaf</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>When your nails accidentally match with things around your house</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6gaaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1e6g84j</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Good putty gels for gel x?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6g84j/good_putty_gels_for_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1e6g24d</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>builder gel w stickers ^_^</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alpbtz6y3bdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1e6fzyf</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Wanted to try the orange nails I’ve been seeing everywhere! 🍊</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afqahzai3bdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1e6fqc9</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>I became addicted to embossed nails🐍🤍</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjx2cmhn1bdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1e6esqd</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>water lily nail !!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3tx8gaotadd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1e6eg4l</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>The simplest I’ve done has become my fave ✨</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1ogwiv3radd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1e6een4</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Comic Con Nails </t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6een4</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1e6dzx8</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>My fresh nails)</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6dzx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1e6demj</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Finally mastered builder gel</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6demj</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1e6cxqa</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Any purple lovers in here? 💜</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gumu3ddyfadd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1e6ct5h</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Glad these turned out pretty nicely 🙏🏼😭</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6ct5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1e6cobc</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Gel Polish Brands</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e6cobc/gel_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1e6cdau</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>I love this coulor !!!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/250z8cnmbadd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1e6cch4</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Another cute self adhesive nail set for $7.</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6cch4</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1e6bopw</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Girl ghost nails</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6bopw</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1e6b1or</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nails (design) go well with this dress? </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8fcwhg01add1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1e69f0e</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just had to hop on the newest 3d flower trend </t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4zs6xdbm9dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1e689c3</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Are press on nails supposed to be uncomfortable?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e689c3/are_press_on_nails_supposed_to_be_uncomfortable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1e66gv2</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>obsessed</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oljqe4b0o8dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1e6xhzs</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Does anybody else get emotionally attached to their pedi color?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6xhzs/does_anybody_else_get_emotionally_attached_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1e6we4c</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Introducing the RL Nail Polish Release Calendar!!</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://sites.google.com/view/nailpolishreleasecalendar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1e6v26o</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Here's your reminder to protect the bees 🐝</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1crodoxjedd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1e6uan6</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Treachery is What You Do Best 🦈🫧</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6uan6</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1e6u991</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails and playing a stringed instrument - how do you do it? I’m trying but it never works. </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayob41dtbedd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1e6tt7j</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>HT Never Tide Down and MC Maelstrom go so well together 😍</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wrwsk5i7edd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1e6td12</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Loveee this new polish</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xj94l063edd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1e6t4wb</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>3 week mooncat &gt; fresh mooncat</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6t4wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1e6s8mi</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>ILNP Malibu and Turquoise Water</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6s8mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1e6s2fy</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Chrysocolla</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hyq7l56rddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1e6s1f8</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Fancy Mermaid Chrome Powder from Fancy</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs0xljmwqddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1e6rn50</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Not usually one for pink…</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulx3nlj9nddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1e6rn3g</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One coat wonders and toppers on toppers </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6rn3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1e6rkwv</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Emily De Molly - Distance to the Sun</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6rkwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1e6qp5u</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Fluorite</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6qp5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1e6qgx7</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How often do you do your nails? </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6qgx7/how_often_do_you_do_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1e6ptzg</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Beach nails at the beach 🏖️</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6ptzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1e6pgcn</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Morningtide + Abalone (DVN)😍</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9nk5wo54ddd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1e6pcq4</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Recommendations for a forest green nail polish?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6pcq4/recommendations_for_a_forest_green_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1e6oow0</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>ILNP Opal Sunset is SO SHIFTY!!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6oow0</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1e6ogfr</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Looking for Nail-Aid 3 Minute Artificials</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a6jtho5wcdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1e6nzcq</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>moonflower 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6nzcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1e6ny3e</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alchemy Lacquers solar polish “Luminary” ☀️ ☁️ </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3y7ivl57scdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1e6mrim</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Matched my nails to an outfit for this weekend!</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/005th3mcicdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1e6mmqx</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Free magnetic wand</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6mmqx/free_magnetic_wand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1e6m4iz</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Prototype Swatch - Y'all inspired me!</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6m4iz</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1e6lxbs</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>i have an obsession with magnetic polishes at the moment, here’s my 2 most recent sets with them! (both gel)</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6lxbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1e6kwy2</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Tell me about your favorite pink glowy/shifty polishes!</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6kwy2/tell_me_about_your_favorite_pink_glowyshifty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1e6kw50</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>metallic flakie jelly 🥪</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6kw50</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1e6kizd</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Mishmash En Rose 🐽🌸🎀🩷</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vngy1sis1cdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1e6kbtj</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Watch out for thinner with toluene</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6kbtj</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1e6jjoo</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Help! My wedding is in 3 weeks. Will full coverage tips even work on these wrecked nails??</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6jjoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1e6iv9g</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dupe for lurid's thistle and thorn? </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6iv9g/dupe_for_lurids_thistle_and_thorn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1e6i8jh</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Bluebell vs fairy dust vs flower child</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6i8jh/bluebell_vs_fairy_dust_vs_flower_child/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1e6hehf</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Color suggestions for upcoming vaca </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6hehf/color_suggestions_for_upcoming_vaca/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1e6haml</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Got a new nude</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ww5r682dbdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1e6gzxh</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Dupe for Chemical X</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6gzxh/dupe_for_chemical_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1e6gc7r</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>What do I do?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3ebjy106bdd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1e6f69h</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Morningtide moment ☀️</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6f69h</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1e6c9vj</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Chemical X is gorgeous 🖤❤️🧡💛💚💙💜🩷</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6c9vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1e6c0w1</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Are you missing the American Classics nail treatments that used to be sold at Sally Beauty Supply like Yellow Stopper, Gelous, or Instant Artificials? They’re back! (Kind of)</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6c0w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1e6bvmc</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Let's talk about magnetics! (Are they too much trouble for a beginner?)</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6bvmc/lets_talk_about_magnetics_are_they_too_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1e6am4w</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Topcoat wars! GLISTEN V VIBRANT</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e6am4w/topcoat_wars_glisten_v_vibrant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1e68gfb</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>What is your favourite red polish?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e68gfb/what_is_your_favourite_red_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1e68bx7</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Essie’s jelly line was at my local CVS</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e68bx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1e67wg1</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>8 Photos of the Exact Same Post because I Couldn't Decide Which Thermal Transition was Best 😂</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e67wg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1e67twq</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>🪸🐠🪼 Polishes Used: Polished for Days (Shade: Just Keep Swimming) | Essie (Shade: Good To Go Topcoat)</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e67twq</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1e67sy7</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Polishes Used: OPI (Shade: Sheen Stealer) | Essie (Shade: Good To Go Topcoat)</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e67sy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1e67rfb</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>🇺🇸 Very late Fourth of July nails</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e67rfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1e67p5m</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>🍑 Polishes Used: Zoya (Shade: Rica) | Essie (Shade: Good To Go Topcoat)</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e67p5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1e67a3u</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Time for a fresh start</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e67a3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1e672x8</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Cirque Color Cobalt Jelly</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e672x8/cirque_color_cobalt_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1e66jp1</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Duo of blues</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/v29gnBf</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1e6vc58</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Here's your reminder to protect the bees 🐝</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yllz41xvmedd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1e6t3tr</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Beautiful aurora chroma nails, i love it, by Ig: leilanailsok</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c50it4ek0edd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1e6nih9</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner at nails </t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6nih9</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1e6nfoe</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>What’s your favorite 3D art products/ tools ?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6nfoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1e6md4x</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Only my third time trying gel but having a lot of fun with dipping my toes in the nail art :D</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpasu7ldfcdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1e6lif9</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>first timer here!! some of you helped me make the decision NOT to go to a certain tech, so i changed my appt last minute and LOVE the results! @ballard_pinkpolish</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6lif9</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1e6l41f</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Semi-permanent gel for my mom, how about it?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsvikw316cdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1e6e4ac</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Progress </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b7l1l7noadd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1e6dwpc</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips on nail art (natural nails) </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e6dwpc/tips_on_nail_art_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1e6d4bm</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Thought about doing check pattern but just left as this— my first time trying more full nail art!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6d4bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1e6crr9</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>SpongeBob</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6crr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1e6cq1g</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>improving my technique... What do you think?💄💅</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgmimsmceadd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1e6af1t</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>How to get into doing nails</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e6af1t/how_to_get_into_doing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1e66yz0</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Lemonade x Grapefruit Aperol Spritz</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgtyq6icu8dd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jul 20 08:08:02 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_21.xlsx
+++ b/data/2024_07_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C950"/>
+  <dimension ref="A1:C1123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16583,6 +16583,2948 @@
         </is>
       </c>
     </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1e7qj9f</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkles all the way </t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssqgg6xmrmdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1e7lfm0</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Nail salon cut the sides of my nails</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7lfm0/nail_salon_cut_the_sides_of_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1e7mhbn</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Best pressons with shorter options?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7mhbn/best_pressons_with_shorter_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1e7oyaf</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>New set ‘Punk’ part IV</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7oyaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1e7q32q</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7da16mg1mmdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1e7p6nn</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>My first short mani, trying out a birthday gift shade!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7p6nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1e7p089</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>🩵 Jack and sally nails 🖤</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/auelp6059mdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1e7ouyw</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Aurora nails experiment</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jlcjczqg7mdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1e7osht</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Still a work in progress😏</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7osht</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1e7o801</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Should I bring my own nail polish to get art?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7o801/should_i_bring_my_own_nail_polish_to_get_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1e7o7x9</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Mermaid nails for summer</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1z7nech20mdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1e7o7c3</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>What brand/ established nail tech would recreate these press ones for me?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7o7c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1e7o6xn</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strawberry Nails 🍓 </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4szge2rzldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1e7o6ry</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>I know I’m late, but my Fourth of July nails ❤️💙</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t25cpn5pzldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1e7o4cl</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Maelstrom decanted</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdieibtyyldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1e7nrs6</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Love this shade of blue!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7nrs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1e7nct2</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>The longest I've had my nails so far, loooove the design so much! 🥰😍 Do u like it!?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsaf3ar0qldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1e7nbtq</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Went to a new nail lady and I’m in love.</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib93w8appldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1e7nbtj</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>so proud on these its like my 4th acrylic set (dont judge my poses :,))</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7nbtj</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1e7mjn7</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>I see people asking about Glamnetics</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7mjn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1e7mgj7</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">xoxo </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hcch1mqgldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1e7kuxl</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue berries </t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k64hz4431ldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1e7kp9u</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She likes my new stickers. </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kugs2omzkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1e7ko77</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Are my cuticles really weird?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7ko77</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1e7kmss</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>A moment of silence for the purple French tips I asked for 😪</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7kmss</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1e7ke7h</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Love square frenchies 🩷🌻</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7ke7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1e7kbbz</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Second attempt at simple nail art</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7kbbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1e7k8o4</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Love my nails but butterfly driving me crazy</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cay93yr9vkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1e7k129</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>A man at the farmers market said my nails look like 1970s wallpaper…he’s not wrong…</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvltmxkatkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1e7jwyi</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>First time Nails</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ac67cx68skdd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1e7jf2s</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>I’m in love</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7jf2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1e7jdgj</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing dip </t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnoovoaankdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1e7j7vf</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vacation Nails </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqo9hi6vlkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1e7iwjj</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>one my favorite sets, such a gorgeous color, s/o to my nail tech for helping me choose! 🖤</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7iwjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1e7ij33</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Do yall know if this UV lamp is safe to use?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7ij33/do_yall_know_if_this_uv_lamp_is_safe_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1e7ihqc</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Daisies for summer 🌼</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq4v99hffkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1e7idmt</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how to do french tip nails? </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7idmt/how_to_do_french_tip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1e7hw2r</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>How can I fix this?</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7hw2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1e7hv54</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>New press on nails</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6av0kcgz9kdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1e7ho22</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>My husbands first time doing my Gel X nails (Before/After)</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7ho22</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1e7hlpk</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Started doing my own acrylic nails - any advice on the cuticle area? </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7hlpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1e7hbzw</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>What happens if you just leave shellac?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7hbzw/what_happens_if_you_just_leave_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1e7hc1y</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>I desperately need to do my nails! Does anyone have any “fresh” ideas?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7hc1y/i_desperately_need_to_do_my_nails_does_anyone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1e7gtr3</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>How can I do these on my own??</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vxoqcye1kdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1e7gtq9</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I told my nail girl I wanted winx club themed nails.. she did it 🥰 </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53fvehxe1kdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1e7gjdb</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love when my nails look nice from the side.  My new nail tech is amazing.  </t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnjps5x2zjdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1e7ggys</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Loooove this polish!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7ggys</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1e7g7if</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Nails day😁 I needed this too much, my nails are a little weak, any recommendation?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7g7if</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1e7g419</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>I dunno…</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sr9ewg8lvjdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1e7fj67</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Picnic theme</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7fj67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1e7fi86</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Can't get a photo of how extra these are 🦩🩵🪷</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7fi86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1e7e2cs</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hem8nmeqfjdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1e7drgi</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Mediterranean nails</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8m1qzxehdjdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1e7dad0</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>yellow szn</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd8kerqu9jdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1e7c517</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>ze bra</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7c517</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1e7c8qi</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Can you help me find a dupe for this color?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7c8qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1e7blqr</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Pink french tip with bow charm</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7blqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1e7bfub</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Owls</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7bfub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1e7bepm</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Builder gel, ANC or acrylic?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7bepm/builder_gel_anc_or_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1e7be3r</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Three days til I leave for Mexico!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7be3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1e7b3vs</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>SHANKS PRESS ON SET</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7b3vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1e7b24h</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Disappointed after second appointment </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7b24h/disappointed_after_second_appointment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1e7afen</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails :) </t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mn50rv04oidd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1e7a0gi</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Inspired by u/mel-cora 🥰</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a6zumf1lidd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1e79k5a</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on matching outfit with nails? </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e79k5a/thoughts_on_matching_outfit_with_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1e79djt</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Bright Pink Tips 💓</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e79djt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1e799a0</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>My new set 🥰</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m06q2ulbfidd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1e78xbi</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>French fade never dies🤗</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4uo1rzscidd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1e75v7s</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>If money and practicality were of no concern, what would be some of your dream nail sets?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e75v7s/if_money_and_practicality_were_of_no_concern_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1e714e5</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>So in love!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e714e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1e776u8</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not sure how to achieve water drops, tried it with top coat. First time doing "fruity" design. ^^ any advice is appreciated! </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abu22u2tzhdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1e77np8</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>I tried impress nails, where did I go wrong?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e77np8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1e78czv</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>love my simple aura nails 💗🌸</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qemaakck8idd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1e78bk5</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think [f28] </t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m662cc8a8idd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1e78a7l</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Green cheetah set - matched pedi/mani</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e78a7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1e786ky</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Do you guys like to use full cover tips or half tips on your nails? And why?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e786ky/do_you_guys_like_to_use_full_cover_tips_or_half/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1e77whq</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My acrylics are too long and I’m freaking out </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tcwrs325idd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1e77ed1</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>When “got milk? 🥛” is the first thing that comes to mind with this nail colour 😂💀</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e77ed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1e770dp</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">84 Stunning Pink Red Nails Designs That Sizzle
+</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e770dp/84_stunning_pink_red_nails_designs_that_sizzle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1e74rxs</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Peel of base coat?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e74rxs/peel_of_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1e76mzp</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Nails for my first kpop concert</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e76mzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1e76myu</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(Repost) I don’t know what to do with my nails </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e76myu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1e76klj</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bobs burgers set I did! </t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22fzisq9vhdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1e761q5</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Rainbow Nails</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e761q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1e75w6x</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Should I change nail shape?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv3r0z54qhdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1e75661</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Evil Eye Nails 💙💛🧿</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e75661</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1e74v4j</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Let's go Purple</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w47o2b6ihdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1e74uy1</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>BISCUIT NAILS</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e74uy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1e74p51</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Cracks forming under nail extension and causing breakage in less than 11 days</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e74p51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1e742lj</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Fake nails keep falling off</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6o8vnbwbhdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1e73tz2</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Think after purchasing too many different kinds, I found my jelly nude!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3nvr16x9hdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1e72ssf</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>What nail shape / color would work for my hands?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4ebwa801hdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1e72izk</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24yqqcfjygdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1e725o1</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Tried doing aura nails with blooming gel but it's giving galaxy instead 💙🌌</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e725o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1e71p28</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>What's a good at home kit to get?</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e71p28/whats_a_good_at_home_kit_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1e71nmx</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Letting my nails grow, small and shiny almonds for me 💫</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mir7hq3qgdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1e71fo2</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ocean nails </t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e71fo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1e714r2</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Watercolour Roses</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifsl96ojkgdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1e6zxng</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>how to get nails when you have eaten them already?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wue39zjp6gdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1e6zt0w</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>my nails are short and I love this shade</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdcwluh15gdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1e7q1dw</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Polish Haul July 2024 😀</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/QR59VTy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1e7o6fj</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Maelstrom decanted</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e7o6fj/maelstrom_decanted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1e7nthl</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Are there any places worth looking at to buy indie polish in NYC?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e7nthl/are_there_any_places_worth_looking_at_to_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1e7ngq5</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Colors- Spa Water (GWP from anniv sale) </t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7ngq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1e7najt</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Potion Polish Cactus Grove </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngvx2hqapldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1e7mptk</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Hoot And A Half by DVN </t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7mptk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1e7ml07</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>y’all weren’t lying about the old Cirque brushes. what the hell</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcuxtbe0ildd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1e7lkpg</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Swatched!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tp5fcy038ldd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1e7kojw</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>One of you recommended Voyage Polish and I may have gone overboard 🤭</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7kojw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1e7knhi</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Orca and shark nails</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7knhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1e7kdb1</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>glass slipper nails 🥹💎</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psijr42jwkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1e7k4wy</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Painted Polish Sale Alert</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl86ma7aukdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1e7j8xy</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Got lucky at Winners</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kd0ra5x4mkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1e7j3h7</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Seashell nails 🐚✨</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hfpg27mqkkdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1e7iqhg</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Non-work mani</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtncy8xihkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1e7icsm</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Please ignore any wobbliness, the lighting on this treadmill is too good! Mooncat getting even base, ILNP after hours velvetized with a 10lb horseshoe, and sally hansen quick dry top coat!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lrsgc797ekdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1e7h9sp</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>First time using seche vite, why did this happen?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnvjol1z4kdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1e7h2qv</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Filing down long nails and never looked back!</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e7h2qv/filing_down_long_nails_and_never_looked_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1e7gfzq</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Thinning peel off base coat?</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e7gfzq/thinning_peel_off_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1e7gdne</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>but actually😭</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qv51frrrxjdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1e7g4bt</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Red and black reversed mani :)</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7g4bt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1e7g38t</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When I say this color is gorgeous, I mean this color is GORGEOUS. </t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7g38t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1e7fncj</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>At what point do you call it quits?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7fncj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1e7fch3</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>She’s giving SunnyD</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7fch3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1e764w0</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is buying nail polish so addictive? </t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e764w0/why_is_buying_nail_polish_so_addictive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1e7e2am</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>my vacation nails before they get completely destroyed</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7e2am</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1e7do85</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Looking for a bold red (like photo) that leans more warm!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5o99271ucjdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1e7dkwd</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Clear manicure always peels!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e7dkwd/clear_manicure_always_peels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1e7cn4j</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>papillon ✨</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7cn4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1e7cj95</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Color Wheel Series: Olive/Chartreuse/Lime </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7cj95</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1e7ahqu</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Cutting them down soon</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7ahqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1e7ae1b</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Just deciding on my next mani, do you like shimmer or no shimmer?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/42rn3mftnidd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1e79hqz</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Quicksand</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e79hqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1e79d5d</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Echo Fabulous!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e79d5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1e78xhh</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Blood Moon 🧛</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6olq28hkcidd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1e78ntq</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Singing in the Rain ☔️</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e78ntq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1e78ftl</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>ILNP - Deep Space 🌌</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e78ftl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1e7895w</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Glass Jellyfish is so glowy!!!!</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qtot5ir7idd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1e77pmh</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>I can’t believe it took me this long to get this color because judging by the amount of matchy-ish things I own, I clearly love it</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e77pmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1e77nzh</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for deep purple with blue glitter nail polish options. Prefer something currently available. </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1dn5kp93idd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1e778fh</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>⭐️ so ethereal, it exceeded expectations 💫</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkh8jg750idd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1e772yd</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>How long have you all been painting your nails?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e772yd/how_long_have_you_all_been_painting_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1e76tbg</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Fixed my stained nails by painting butterfly wings over them (yes they are a bit wonky)</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e76tbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1e76lyt</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Love this duo!</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goln0gljvhdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1e76ey4</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Solar Bali Sand</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e76ey4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1e7580l</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>This one got away from me after a few escalating attempts to fix mistakes</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fj7x0aoxkhdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1e74ws3</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Very casual at painting my nails (sorry for the application) and having a hard time figuring out which colors suit my skin tone. What about Essie Lilacism?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e74ws3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1e74p70</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>nailpollies anything is popsicle</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33503pggghdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1e73xee</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Ugly or not? 🟢</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e73xee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1e73nen</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Flakie rainbow skittle</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e73nen</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1e73fzz</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>What are redacted polishes?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e73fzz/what_are_redacted_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1e72qa1</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>See you space cowboy</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e72qa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1e71mxr</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Love this shade of blue, it matches my name 💎</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5nkx3swpgdd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1e71hqy</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Two butterfly polishes!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e71hqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1e70c3q</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Here is your reminder to never forget your base coat</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zh46zshbgdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1e7omss</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Finally got the hang of stamping, so I made some dnd themed nails that change color!</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ndzf8v2v4mdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1e7m5hj</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time making a portrait on a nail </t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uebmxrjpdldd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1e7l7fy</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Second press ons I've ever done!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ld2hl7f4ldd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1e7jxyr</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Black 🖤</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvq7ywnhskdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1e7j198</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first attempt at doing my own nails with overlays eek </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/up3cby27kkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1e7iq8r</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Some of my favorites I’ve done</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7iq8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1e7ih3f</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your opinions on the moon cut shape? </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mms16i9fkdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1e7iejy</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how to do french tip nails? </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e7iejy/how_to_do_french_tip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1e7dk1j</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I think this is my best set yet</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0np6dbybjdd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1e7cafe</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Too Much?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0bpeyi82jdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1e7b0pj</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back to school? I'm getting lady bug vibes instead. </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw71rmklsidd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1e7aasn</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Rubber Base. 💜</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqam2lw4nidd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1e78el2</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Did my own nails for my wedding</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e78el2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1e78c2x</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Green cheetah set - matched mani/pedi</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e78c2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1e75je0</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Still Looking For a Perfect Ethereal Pink, attempt 2</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvplyr6fnhdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1e71jv3</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6jiitm0pgdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1e6zk9e</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Lenticular nail art</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e6zk9e/lenticular_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1e6zh1q</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Summer nails before holidays! How does it look?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6egx486v0gdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jul 21 08:08:11 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_21.xlsx
+++ b/data/2024_07_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1123"/>
+  <dimension ref="A1:C1294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19525,6 +19525,2913 @@
         </is>
       </c>
     </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1e8h9zl</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>My nailz</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0y3xmkhwtdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1e8h3xu</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>This week's silver chrome summerween set, featuring my nail inspector Speckles</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pyzprk65utdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1e8h2i3</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Well this happened to me 😭</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hznnyabsttdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1e8ekch</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel/methacrylate/HEMA allergy presentation? </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e8ekch/gelmethacrylatehema_allergy_presentation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1e8bpqb</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Thinking of going from shellac to dip. What are some pros/ cons?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f10nufmw5sdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1e8cmti</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Can anyone tell me what these nail tools are for?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8cmti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1e8cvjo</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail injury </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e8cvjo/nail_injury/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1e8eo7b</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo Taco has saved me during gel allergy </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ob4anj11tdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1e8f7kh</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>PopUpNails Mean Girl Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8m78mok87tdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1e8c2so</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8c2so</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1e8c2nc</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>How do you girls do stuff with long\short nails?</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e8c2nc/how_do_you_girls_do_stuff_with_longshort_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1e8fjyl</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Pink is my favorite🎀</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8fjyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1e8fjf3</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>first time getting my nails done 🥹</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8fjf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1e8fea3</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>my nail broke on the side is it a bad idea to let it grow out? should i just file it down?</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50f392ch9tdd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1e8ew0i</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>New nails yayy reminds me of bubble gum</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8ew0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1e8ejqi</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I did today </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9v9beqvnzsdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1e8e8es</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Fill or Whole New Manicure?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e8e8es/fill_or_whole_new_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1e8dxzv</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Got my first set in a salon and…</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e8dxzv/got_my_first_set_in_a_salon_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1e8dqu4</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Felt like trimming them</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8dqu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1e8d7jv</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Opalite to match my wedding stone ♡</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8d7jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1e8d1jv</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Isn't red too tempting?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32rmtxb0jsdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1e8c2c6</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>I love nail days</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0hacvx99sdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1e8butj</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>New presson set 😊</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8butj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1e8bs4t</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Opals ✨️</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8bs4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1e8bo9s</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Yayyy You’re here 2024</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8bo9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1e8b98h</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>The Olympics are coming!</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8b98h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1e8b4fu</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time french tip :) </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8b4fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1e8aedo</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Beauty &amp; the Beast inspired nails for a good reason...</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8aedo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1e8axw2</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freshly made 😍 </t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln0x95t5yrdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1e89qs0</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Made my own press ons today!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ch098hwmrdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1e8amgw</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>First time getting nail art!</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8amgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1e8akko</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Jelly Glue</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e8akko/jelly_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1e8a8ht</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Sunflowers🌻</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46td6w7errdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1e8a2rw</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Kiss Impress press ons. They last 1-2 weeks and take 5 minutes.</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytfs0onxprdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1e89yud</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Asked for something black</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu71pikwordd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1e89q6u</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does this colour suit me? </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbp9sqzqmrdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1e869q0</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Some nail inspiration for you all</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e869q0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1e88v18</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">got acrylics for the first time and i’m IN LOVE </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw73yii4frdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1e88tv5</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>🤎🐢</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tacdq9zxcrdd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1e88btm</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a tragedy 😭 </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i5w8fimardd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1e887lc</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Hibiscus French Tips</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve5pfg9n9rdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1e886kr</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Do yall like 😌?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e886kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1e880lz</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>First time trying sheer! I’m in love!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ermek1u18rdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1e87xly</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Just wanted to share my newest set</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e87xly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1e87i8b</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Any Jujutsu Kaisen fans?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pdcostq3rdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1e87d75</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Butter </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uilxx0vj2rdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1e87d4w</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Is there a way to stop nicotine stains?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lvm17cj2rdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1e87atf</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>What would you pay?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e87atf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1e87ais</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Just wanted to post my laat nails colors before i change them with another one~</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e87ais</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1e86yh9</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Jade nails 🌿🐉</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e86yh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1e86x89</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just a beginner </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e86x89</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1e86nok</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>My wedding nails from last week 🥰</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e86nok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1e86hm4</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any advice on how to get the clean girl short nail look? Just got these done. </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfqw60g1vqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1e867lq</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Obsessed with Summer nails!!</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e867lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1e8658y</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzzeufz3sqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1e85yfs</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Loving the brightness of this soft pink</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e85yfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1e85ye0</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Watermelon summer... &amp; a few others</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e85ye0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1e85sl7</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Chrome nails</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e85sl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1e7vjuw</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Why do my cuticles do this after I get my nails done?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/juj5xia9dodd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1e7yb9u</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time here what do I do? </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2irg6dzc0pdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1e85onl</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I kinda miss scratching myself with the long n pointy nails </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3r2nyd6oqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1e84t79</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>My new claws!!!! Inspo by @quaynaildit on IG</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e84t79</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1e85o7r</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Lamp for casual user</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e85o7r/lamp_for_casual_user/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1e84yjw</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Show off your squoval nails!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e84yjw/show_off_your_squoval_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1e84yly</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Are my nails just too sensitive for extensions/polishes of any kind? Is that a known condition?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e84yly/are_my_nails_just_too_sensitive_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1e85ezm</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Sweltering</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yza2z3fylqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1e853k7</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>I don't even know what to say.</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e853k7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1e84u74</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>What shape/color do you think looks best?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e84u74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1e84sdz</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Trying out new nail polish.</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e84sdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1e84rvm</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Goamnetics usually last 2-3 weeks for me.. any other brands do this?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e84rvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1e84mu2</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>First time 🍊 what do you think?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e84mu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1e84j3x</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Men allowed in this subreddit? Because I love these and wanted others to see.</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rx4xdz1meqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1e84cmw</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Pink sunset aura nails (on apres gel-x)</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e84cmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1e84gf4</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>New to painting press ons</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e84gf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1e84gb4</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Really happy with these (plz ignore the dog hair)</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e84gb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1e84g5e</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Is it necessary to remove the cuticle?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpucd0dydqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1e7yhlc</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>wildflower nails!</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyel56nq1pdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1e7yuyw</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pastel butterflys </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/qOTEhjIWQlI?si=s8jwhXG_Z_2z7O03</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1e7yxbk</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bow nails </t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/13xB4Pkhh7w?si=mHeD0NyHxJlNWZ-v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1e80gdi</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Summer French! What’s the verdict?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e80gdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1e836mp</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you guys get rid of the thick skin around the nail? Not Cuticle but actual skin on your finger. I was using the Kerasal ointment but it's not strong enough. Any suggestions or tips would be SO Very appreciated. </t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e836mp/how_do_you_guys_get_rid_of_the_thick_skin_around/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1e7tyld</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Are these nails too chunky?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7tyld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1e7s6z5</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>which nails should i get?? (photos from picturehouseee on pinterest)</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7s6z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1e7rr39</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>How to get out of a nail funk?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e7rr39/how_to_get_out_of_a_nail_funk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1e83yh7</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>cutie star girl nails i did on my bestie⭐️🍓</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e83yh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1e83u0f</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Probably my fav set so far 💜</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/csr6s8hw8qdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1e83c5l</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How are feeling about the duck nails coming back in trend ? </t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e83c5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1e82yg7</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>I think this is my favorite set in this year :)</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pyx93xq1qdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1e82xiv</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>I screamed</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfp84omj1qdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1e82jzy</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Almond or round on me? (XS length)</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e82jzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1e82dus</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Did my mom’s nails for her birthday, I love her so much!🥹 Pink with a flower canopy</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/on8gzmi3xpdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1e8276n</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">alrighty so I got some hard gel extensions, and I love the length so much. my natural nails are still pretty long underneath </t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjuuq95lvpdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1e81vn4</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best manicure type for vacation? </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e81vn4/best_manicure_type_for_vacation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1e81khf</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>I don’t know what colour to do ;(</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e81khf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1e816w3</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pierre and I modeling Cirque Colors Madder </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e816w3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1e81236</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Press on nails for the win!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dxq3v0dmpdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1e80yvl</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some designs I’ve had ☺️❤️ </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e80yvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1e80vdn</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>What do y’all think?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au5nvkbukpdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1e80avg</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Is it normal for gel x nails to randomly pop off?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sizixv5bgpdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1e803tk</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Rainbow ombré chromies for pride events this weekend🌈✨🫧</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ts24szvqepdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1e8h9er</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Favorite alternative to Kerasal?</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e8h9er/favorite_alternative_to_kerasal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1e8h1vo</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Anyone know of a dupe for Starrily's Stargazer by Kelli Marissa?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cde7wjkttdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1e8fnap</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>changed my nail shape for the first time in 8 years</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k63fabafctdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1e8f9hm</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Protecting layer under nail glue? </t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e8f9hm/protecting_layer_under_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1e8ewh8</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>A moment of silence for my nails</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8ewh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1e8czoi</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which is your favorite nail to have be the feature nail? Or which two, if that's your MO? I'm an A&amp;C gal myself </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8czoi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1e8coha</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>This weekend’s at-home mani</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb2qqnfefsdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1e8c8pz</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Pumpkin in July</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8c8pz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1e8bmyj</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Yayyy You’re here 2024</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8bmyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1e8blso</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Enjoying Dark Horse</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8blso</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1e8bf7f</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Question about Holo Taco / thermals collection</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e8bf7f/question_about_holo_taco_thermals_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1e8baem</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Road Rage</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8baem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1e8aqgq</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>EA Sports. It’s in the Game!</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8aqgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1e829yb</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Where can I find this jelly nail polish?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e829yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1e86v7n</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Gel X</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e86v7n/gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1e8980d</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Kiss nail dress strips?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e8980d/kiss_nail_dress_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1e88ee9</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Has anyone ever tried these modelones jelly polishes?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh7rchs7brdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1e888ja</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>🦋and way up there, i actually love it🦋</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypeglzev9rdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1e86t9b</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Trying out a new combo!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbm7y9rtxqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1e86fci</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Need recommendations for weak nails</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e86fci/need_recommendations_for_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1e86apl</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>My Cirque Colors Lucky Bag! 🍀</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwha8xydtqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1e85zw1</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>What nail polish brands work well with the Sally Hansen lamp?</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e85zw1/what_nail_polish_brands_work_well_with_the_sally/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1e85ie2</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tiny KB Shimmer haul </t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e85ie2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1e853sa</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>✨Sunset dust✨</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e853sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1e83zwh</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Another Am I Everything You Fear fan</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e83zwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1e83nwt</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Probably my fav set so far 💜</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dp5ukgpi7qdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1e833ck</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Recommendations to match?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80xziwwu2qdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1e82x1j</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arcana - My Life As a Shrimp </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e82x1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1e81di6</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Little blue and big blue</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2w1p6vxopdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1e816tx</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Accidentally matched nails with my spoon</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6girhisgnpdd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1e80w4f</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Customer Service </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yojx6ps0lpdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1e809vr</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Stars Above</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e809vr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1e7yrth</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Olives and Mustard</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7yrth</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1e7xkpj</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Accidentally but perfectly matched my clothes to my polish the other day 😍 I love when that happens</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1hnu0oguodd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1e7xhn1</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Louisiana by Magpie</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7xhn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1e7xhgc</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>DVN- Strawberry In A Jam 🍓</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7xhgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1e7wu01</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>My version of Baccarat nails, and the $1,200 inspo</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7wu01</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1e7wrvf</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Opi bubble bath and brush lines</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e7wrvf/opi_bubble_bath_and_brush_lines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1e7w8qq</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Recommendations please! :)</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e7w8qq/recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1e7vthw</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Pink + black = blue???</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7vthw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1e7vlrl</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Daisy Chain Polish Skittle and 16% Off Sale</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7vlrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1e7usi1</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">All of the polish I have found for free in the past month. Storytime! </t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7usi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1e7unnv</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Shining like gemstones! 💎</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7unnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1e7u6ng</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My partner let me do her nails </t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7u6ng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1e7tkl0</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Forever trying to capture how beautiful this polish is</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7tkl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1e8f3wq</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8f3wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1e8el40</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>What I did today</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7s9b8s30tdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1e8dmdd</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>How are these nails ive done?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8dmdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1e8d2gt</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>What are these nail tools for??</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8d2gt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1e8btvu</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New press on set </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8btvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1e8bohf</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>coraline nails!</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsqh3foj5sdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1e8ad6l</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art </t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l06q2v9msrdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1e89ojz</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished my first goth/alternative set for my friend! :) </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puhbrlhcmrdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1e89l0w</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Best brushes for nail art? My lines always come out thick :(</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6j2bwbflrdd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1e88zuu</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>My first hand painted set!</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfj73fm9grdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1e87sjw</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The longest I've had my nails so far! </t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e87sjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1e87lc2</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Any Jujutsu Kaisen fans?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26d2xs4g4rdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1e872rk</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Hand painted tiny insects nail art</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6a0r6d30rdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1e86k9r</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Attempt at simple Koi nails🫧</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e86k9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1e86k93</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b67y45sovqdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1e86ern</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>🪽</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/525aulqcuqdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1e8687g</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Obsessed With Summer Nails!!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e8687g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1e845tw</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>I can't decide if it's galaxy or ocean vibes💙</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/71b8g0zkbqdd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1e81o87</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>My practice attempts at gemstone inspired nails 😁(ignore my dirty mat) 🫣</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e81o87</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1e80c9q</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>a friend made them for me</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ds478ytmgpdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1e7z8ar</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7z8ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1e7y4f4</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>First set of gel nails I got</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dwvtliuyodd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1e7wdt1</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made by me @streetnailart ig </t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7ohgp1kkodd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1e7w444</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Topcoat flooding cuticles!! Pls help advice needed </t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yh5dxll9iodd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1e7smip</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swan lake </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e7smip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1e7r8b1</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>My new sets of design 🥰</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/my53a0wi0ndd1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>